<commit_message>
Error volume plot, much moving around in front part of paper.
</commit_message>
<xml_diff>
--- a/calibration/axis_stats_cal_9_16_premo_rotated_dipole.xlsx
+++ b/calibration/axis_stats_cal_9_16_premo_rotated_dipole.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DF87BB-B6E9-4DD8-927E-2C1306FA7514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B669EA-219A-4783-8639-1D18D888275B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="4068" windowWidth="17820" windowHeight="9408" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="34560" windowHeight="19140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="by axis" sheetId="1" r:id="rId1"/>
@@ -361,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -535,6 +535,81 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -580,21 +655,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -610,91 +670,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -702,7 +682,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1054,28 +1057,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="92" t="s">
+      <c r="C2" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="93"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="95" t="s">
+      <c r="D2" s="120"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="96"/>
-      <c r="H2" s="97"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="124"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C3" s="21" t="s">
@@ -1098,7 +1101,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="105" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1124,7 +1127,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="99"/>
+      <c r="A5" s="105"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1148,7 +1151,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="105" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1174,7 +1177,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="99"/>
+      <c r="A7" s="105"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1198,7 +1201,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="99" t="s">
+      <c r="A8" s="105" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1224,7 +1227,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="99"/>
+      <c r="A9" s="105"/>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1248,7 +1251,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="99" t="s">
+      <c r="A10" s="105" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1274,7 +1277,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="99"/>
+      <c r="A11" s="105"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1320,40 +1323,40 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="87"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="89" t="s">
+      <c r="D13" s="114"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="90"/>
-      <c r="H13" s="91"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="118"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="106" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="98"/>
-      <c r="H15" s="98"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="106"/>
+      <c r="F15" s="106"/>
+      <c r="G15" s="106"/>
+      <c r="H15" s="106"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
-      <c r="C16" s="100" t="s">
+      <c r="C16" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="101"/>
-      <c r="E16" s="102"/>
-      <c r="F16" s="100" t="s">
+      <c r="D16" s="108"/>
+      <c r="E16" s="109"/>
+      <c r="F16" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="101"/>
-      <c r="H16" s="102"/>
+      <c r="G16" s="108"/>
+      <c r="H16" s="109"/>
     </row>
     <row r="17" spans="1:16377" x14ac:dyDescent="0.3">
       <c r="C17" s="33" t="s">
@@ -1376,7 +1379,7 @@
       </c>
     </row>
     <row r="18" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A18" s="99" t="s">
+      <c r="A18" s="105" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1412,7 +1415,7 @@
       <c r="T18" s="13"/>
     </row>
     <row r="19" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A19" s="99"/>
+      <c r="A19" s="105"/>
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1446,7 +1449,7 @@
       <c r="T19" s="13"/>
     </row>
     <row r="20" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A20" s="99" t="s">
+      <c r="A20" s="105" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1482,7 +1485,7 @@
       <c r="T20" s="13"/>
     </row>
     <row r="21" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A21" s="99"/>
+      <c r="A21" s="105"/>
       <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
@@ -17873,7 +17876,7 @@
       <c r="XEW21" s="13"/>
     </row>
     <row r="22" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A22" s="99" t="s">
+      <c r="A22" s="105" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -17909,7 +17912,7 @@
       <c r="T22" s="13"/>
     </row>
     <row r="23" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A23" s="99"/>
+      <c r="A23" s="105"/>
       <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
@@ -17943,7 +17946,7 @@
       <c r="T23" s="13"/>
     </row>
     <row r="24" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A24" s="99" t="s">
+      <c r="A24" s="105" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -34338,7 +34341,7 @@
       <c r="XEW24" s="13"/>
     </row>
     <row r="25" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A25" s="99"/>
+      <c r="A25" s="105"/>
       <c r="B25" s="1" t="s">
         <v>4</v>
       </c>
@@ -50752,16 +50755,16 @@
       </c>
     </row>
     <row r="27" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="C27" s="83" t="s">
+      <c r="C27" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="84"/>
-      <c r="E27" s="85"/>
-      <c r="F27" s="83" t="s">
+      <c r="D27" s="111"/>
+      <c r="E27" s="112"/>
+      <c r="F27" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="84"/>
-      <c r="H27" s="85"/>
+      <c r="G27" s="111"/>
+      <c r="H27" s="112"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
@@ -50787,6 +50790,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="C15:H15"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="A18:A19"/>
@@ -50798,13 +50808,6 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="C15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -50828,14 +50831,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="128" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="107"/>
-      <c r="E1" s="106" t="s">
+      <c r="D1" s="129"/>
+      <c r="E1" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="107"/>
+      <c r="F1" s="129"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" s="54" t="s">
@@ -50860,13 +50863,13 @@
       <c r="D3" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="103" t="s">
+      <c r="E3" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="104"/>
+      <c r="F3" s="126"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="127" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="52" t="s">
@@ -50886,7 +50889,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="105"/>
+      <c r="A5" s="127"/>
       <c r="B5" s="52" t="s">
         <v>19</v>
       </c>
@@ -50904,7 +50907,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="105" t="s">
+      <c r="A6" s="127" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="52" t="s">
@@ -50924,7 +50927,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="105"/>
+      <c r="A7" s="127"/>
       <c r="B7" s="52" t="s">
         <v>19</v>
       </c>
@@ -50942,7 +50945,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="105" t="s">
+      <c r="A8" s="127" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="52" t="s">
@@ -50962,7 +50965,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="105"/>
+      <c r="A9" s="127"/>
       <c r="B9" s="52" t="s">
         <v>19</v>
       </c>
@@ -50980,7 +50983,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="105" t="s">
+      <c r="A10" s="127" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="52" t="s">
@@ -51000,7 +51003,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="105"/>
+      <c r="A11" s="127"/>
       <c r="B11" s="52" t="s">
         <v>19</v>
       </c>
@@ -51051,13 +51054,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.21875" style="110" customWidth="1"/>
+    <col min="1" max="1" width="5.21875" style="83" customWidth="1"/>
     <col min="2" max="2" width="3.77734375" style="72" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="5.44140625" style="73" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.44140625" style="73" bestFit="1" customWidth="1"/>
@@ -51065,35 +51068,35 @@
     <col min="7" max="16384" width="8.88671875" style="73"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="140" customFormat="1" ht="10.8" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="136"/>
-      <c r="B1" s="137"/>
-      <c r="C1" s="138" t="s">
+    <row r="1" spans="1:6" s="104" customFormat="1" ht="10.8" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="102"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="139"/>
-      <c r="E1" s="138" t="s">
+      <c r="D1" s="133"/>
+      <c r="E1" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="139"/>
+      <c r="F1" s="136"/>
     </row>
-    <row r="2" spans="1:6" s="127" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="110"/>
-      <c r="B2" s="125"/>
+    <row r="2" spans="1:6" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="83"/>
+      <c r="B2" s="92"/>
       <c r="C2" s="74" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="126" t="s">
+      <c r="E2" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="75" t="s">
+      <c r="F2" s="137" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="127" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="94" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="76"/>
       <c r="B3" s="77"/>
       <c r="C3" s="81" t="s">
@@ -51102,116 +51105,116 @@
       <c r="D3" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="108" t="s">
+      <c r="E3" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="109"/>
+      <c r="F3" s="141"/>
     </row>
-    <row r="4" spans="1:6" s="127" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="111" t="s">
+    <row r="4" spans="1:6" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="131" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="114">
+      <c r="C4" s="84">
         <f>combined!C8</f>
         <v>0.10375520670237465</v>
       </c>
-      <c r="D4" s="115">
+      <c r="D4" s="85">
         <f>combined!D8</f>
         <v>0.22660354611847008</v>
       </c>
-      <c r="E4" s="128">
+      <c r="E4" s="95">
         <f>combined!E8</f>
         <v>3.8505200114367184E-3</v>
       </c>
-      <c r="F4" s="116">
+      <c r="F4" s="95">
         <f>combined!F8</f>
         <v>4.4292861800983895E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="127" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="112"/>
+    <row r="5" spans="1:6" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="135"/>
       <c r="B5" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="114">
+      <c r="C5" s="84">
         <f>combined!C9</f>
         <v>0.19014646862512824</v>
       </c>
-      <c r="D5" s="115">
+      <c r="D5" s="85">
         <f>combined!D9</f>
         <v>0.40759885006830154</v>
       </c>
-      <c r="E5" s="128">
+      <c r="E5" s="95">
         <f>combined!E9</f>
         <v>6.8924055315988768E-3</v>
       </c>
-      <c r="F5" s="116">
+      <c r="F5" s="95">
         <f>combined!F9</f>
         <v>6.6501541883260675E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="127" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="113" t="s">
+    <row r="6" spans="1:6" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="130" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="117">
+      <c r="C6" s="86">
         <f>combined!C10</f>
         <v>0.13931184780921721</v>
       </c>
-      <c r="D6" s="118">
+      <c r="D6" s="87">
         <f>combined!D10</f>
         <v>9.4700747159384382E-2</v>
       </c>
-      <c r="E6" s="119">
+      <c r="E6" s="88">
         <f>combined!E10</f>
         <v>2.973307566157643E-3</v>
       </c>
-      <c r="F6" s="120">
+      <c r="F6" s="138">
         <f>combined!F10</f>
         <v>4.9683053200820209E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="127" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="111"/>
+    <row r="7" spans="1:6" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="131"/>
       <c r="B7" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="121">
+      <c r="C7" s="89">
         <f>combined!C11</f>
         <v>0.22384620596603561</v>
       </c>
-      <c r="D7" s="122">
+      <c r="D7" s="90">
         <f>combined!D11</f>
         <v>0.17398206651153414</v>
       </c>
-      <c r="E7" s="123">
+      <c r="E7" s="91">
         <f>combined!E11</f>
         <v>3.3215777674644661E-3</v>
       </c>
-      <c r="F7" s="124">
+      <c r="F7" s="139">
         <f>combined!F11</f>
         <v>9.2371917699481752E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="135" customFormat="1" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="129"/>
-      <c r="B8" s="130"/>
-      <c r="C8" s="131" t="s">
+    <row r="8" spans="1:6" s="101" customFormat="1" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="96"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="132" t="s">
+      <c r="D8" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="133" t="s">
+      <c r="E8" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="134" t="s">
+      <c r="F8" s="140" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Progressive refinement of calibration paper, added residue_stats.xlsx
</commit_message>
<xml_diff>
--- a/calibration/axis_stats_cal_9_16_premo_rotated_dipole.xlsx
+++ b/calibration/axis_stats_cal_9_16_premo_rotated_dipole.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B669EA-219A-4783-8639-1D18D888275B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF56C71-5D23-41E3-A167-DBADE232D20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="34560" windowHeight="19140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="34560" windowHeight="19140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="by axis" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="31">
   <si>
     <t>On axis</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>RxRyRz</t>
-  </si>
-  <si>
-    <t>RzRyRz</t>
   </si>
   <si>
     <t>RxRyRx</t>
@@ -595,20 +592,17 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -655,6 +649,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -682,29 +691,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1057,28 +1054,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="119" t="s">
+      <c r="C2" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="120"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="122" t="s">
+      <c r="D2" s="119"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="123"/>
-      <c r="H2" s="124"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="123"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C3" s="21" t="s">
@@ -1101,7 +1098,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="125" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1127,7 +1124,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="105"/>
+      <c r="A5" s="125"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1151,7 +1148,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="105" t="s">
+      <c r="A6" s="125" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1177,7 +1174,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="105"/>
+      <c r="A7" s="125"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1201,7 +1198,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="105" t="s">
+      <c r="A8" s="125" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1227,7 +1224,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="105"/>
+      <c r="A9" s="125"/>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1251,7 +1248,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="105" t="s">
+      <c r="A10" s="125" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1277,7 +1274,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="105"/>
+      <c r="A11" s="125"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1323,40 +1320,40 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="C13" s="113" t="s">
+      <c r="C13" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="114"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="116" t="s">
+      <c r="D13" s="113"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="117"/>
-      <c r="H13" s="118"/>
+      <c r="G13" s="116"/>
+      <c r="H13" s="117"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C15" s="106" t="s">
+      <c r="C15" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="106"/>
+      <c r="D15" s="124"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
-      <c r="C16" s="107" t="s">
+      <c r="C16" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="108"/>
-      <c r="E16" s="109"/>
-      <c r="F16" s="107" t="s">
+      <c r="D16" s="127"/>
+      <c r="E16" s="128"/>
+      <c r="F16" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="108"/>
-      <c r="H16" s="109"/>
+      <c r="G16" s="127"/>
+      <c r="H16" s="128"/>
     </row>
     <row r="17" spans="1:16377" x14ac:dyDescent="0.3">
       <c r="C17" s="33" t="s">
@@ -1379,7 +1376,7 @@
       </c>
     </row>
     <row r="18" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A18" s="105" t="s">
+      <c r="A18" s="125" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1415,7 +1412,7 @@
       <c r="T18" s="13"/>
     </row>
     <row r="19" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A19" s="105"/>
+      <c r="A19" s="125"/>
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1449,7 +1446,7 @@
       <c r="T19" s="13"/>
     </row>
     <row r="20" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A20" s="105" t="s">
+      <c r="A20" s="125" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1485,7 +1482,7 @@
       <c r="T20" s="13"/>
     </row>
     <row r="21" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A21" s="105"/>
+      <c r="A21" s="125"/>
       <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
@@ -17876,7 +17873,7 @@
       <c r="XEW21" s="13"/>
     </row>
     <row r="22" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A22" s="105" t="s">
+      <c r="A22" s="125" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -17912,7 +17909,7 @@
       <c r="T22" s="13"/>
     </row>
     <row r="23" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A23" s="105"/>
+      <c r="A23" s="125"/>
       <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
@@ -17946,7 +17943,7 @@
       <c r="T23" s="13"/>
     </row>
     <row r="24" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A24" s="105" t="s">
+      <c r="A24" s="125" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -34341,7 +34338,7 @@
       <c r="XEW24" s="13"/>
     </row>
     <row r="25" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A25" s="105"/>
+      <c r="A25" s="125"/>
       <c r="B25" s="1" t="s">
         <v>4</v>
       </c>
@@ -50755,16 +50752,16 @@
       </c>
     </row>
     <row r="27" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="C27" s="110" t="s">
+      <c r="C27" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="111"/>
-      <c r="E27" s="112"/>
-      <c r="F27" s="110" t="s">
+      <c r="D27" s="110"/>
+      <c r="E27" s="111"/>
+      <c r="F27" s="109" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="111"/>
-      <c r="H27" s="112"/>
+      <c r="G27" s="110"/>
+      <c r="H27" s="111"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
@@ -50790,13 +50787,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="C15:H15"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="A18:A19"/>
@@ -50808,6 +50798,13 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="C15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -50831,21 +50828,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C1" s="128" t="s">
+      <c r="C1" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="129"/>
-      <c r="E1" s="128" t="s">
+      <c r="D1" s="133"/>
+      <c r="E1" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="129"/>
+      <c r="F1" s="133"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" s="54" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="55" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="56" t="s">
         <v>17</v>
@@ -50863,13 +50860,13 @@
       <c r="D3" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="125" t="s">
+      <c r="E3" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="126"/>
+      <c r="F3" s="130"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="131" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="52" t="s">
@@ -50889,7 +50886,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="127"/>
+      <c r="A5" s="131"/>
       <c r="B5" s="52" t="s">
         <v>19</v>
       </c>
@@ -50907,7 +50904,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="127" t="s">
+      <c r="A6" s="131" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="52" t="s">
@@ -50927,7 +50924,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="127"/>
+      <c r="A7" s="131"/>
       <c r="B7" s="52" t="s">
         <v>19</v>
       </c>
@@ -50945,7 +50942,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="127" t="s">
+      <c r="A8" s="131" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="52" t="s">
@@ -50965,7 +50962,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="127"/>
+      <c r="A9" s="131"/>
       <c r="B9" s="52" t="s">
         <v>19</v>
       </c>
@@ -50983,7 +50980,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="127" t="s">
+      <c r="A10" s="131" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="52" t="s">
@@ -51003,7 +51000,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="127"/>
+      <c r="A11" s="131"/>
       <c r="B11" s="52" t="s">
         <v>19</v>
       </c>
@@ -51029,7 +51026,7 @@
         <v>14</v>
       </c>
       <c r="E12" s="54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" s="71" t="s">
         <v>18</v>
@@ -51055,7 +51052,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:F3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -51071,14 +51068,14 @@
     <row r="1" spans="1:6" s="104" customFormat="1" ht="10.8" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A1" s="102"/>
       <c r="B1" s="103"/>
-      <c r="C1" s="132" t="s">
+      <c r="C1" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="133"/>
-      <c r="E1" s="132" t="s">
+      <c r="D1" s="137"/>
+      <c r="E1" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="136"/>
+      <c r="F1" s="138"/>
     </row>
     <row r="2" spans="1:6" s="94" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="83"/>
@@ -51092,8 +51089,8 @@
       <c r="E2" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="137" t="s">
-        <v>29</v>
+      <c r="F2" s="105" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="94" customFormat="1" x14ac:dyDescent="0.2">
@@ -51105,13 +51102,13 @@
       <c r="D3" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="134" t="s">
+      <c r="E3" s="139" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="141"/>
+      <c r="F3" s="140"/>
     </row>
     <row r="4" spans="1:6" s="94" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="131" t="s">
+      <c r="A4" s="135" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="79" t="s">
@@ -51135,7 +51132,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="94" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="135"/>
+      <c r="A5" s="141"/>
       <c r="B5" s="80" t="s">
         <v>19</v>
       </c>
@@ -51157,7 +51154,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="94" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="130" t="s">
+      <c r="A6" s="134" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="82" t="s">
@@ -51175,13 +51172,13 @@
         <f>combined!E10</f>
         <v>2.973307566157643E-3</v>
       </c>
-      <c r="F6" s="138">
+      <c r="F6" s="106">
         <f>combined!F10</f>
         <v>4.9683053200820209E-3</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="94" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="131"/>
+      <c r="A7" s="135"/>
       <c r="B7" s="79" t="s">
         <v>19</v>
       </c>
@@ -51197,7 +51194,7 @@
         <f>combined!E11</f>
         <v>3.3215777674644661E-3</v>
       </c>
-      <c r="F7" s="139">
+      <c r="F7" s="107">
         <f>combined!F11</f>
         <v>9.2371917699481752E-3</v>
       </c>
@@ -51212,9 +51209,9 @@
         <v>14</v>
       </c>
       <c r="E8" s="100" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
-      <c r="F8" s="140" t="s">
+      <c r="F8" s="108" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>